<commit_message>
make sure URNs are unchanged
compat mode 1 with small fix in convert_library for skip feature
</commit_message>
<xml_diff>
--- a/tools/excel/dora/dora_new.xlsx
+++ b/tools/excel/dora/dora_new.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/dora/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA863BDD-77B5-4244-A617-7B0A9DA5FAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0817F4F3-0D10-4F44-BA45-5272E58AA4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
     <sheet name="dora_meta" sheetId="2" r:id="rId2"/>
     <sheet name="dora_content" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dora_content!$A$1:$L$683</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -12684,7 +12687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" workbookViewId="0">
+    <sheetView zoomScale="220" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -12978,8 +12981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L700"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E377" sqref="E377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15699,7 +15702,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
       <c r="B109" s="5">
         <v>1</v>
@@ -15730,7 +15733,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="6"/>
       <c r="B110" s="5">
         <v>2</v>
@@ -15811,7 +15814,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A113" s="6"/>
       <c r="B113" s="5">
         <v>3</v>
@@ -15892,7 +15895,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="270" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A116" s="6"/>
       <c r="B116" s="5">
         <v>3</v>
@@ -15965,7 +15968,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="6"/>
       <c r="B119" s="5">
         <v>2</v>
@@ -16021,7 +16024,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
       <c r="B121" s="5">
         <v>3</v>
@@ -16146,7 +16149,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" ht="195" x14ac:dyDescent="0.2">
       <c r="A126" s="6"/>
       <c r="B126" s="5">
         <v>3</v>
@@ -16221,7 +16224,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="384" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A129" s="6"/>
       <c r="B129" s="5">
         <v>3</v>
@@ -16246,7 +16249,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A130" s="6"/>
       <c r="B130" s="5">
         <v>3</v>
@@ -16271,7 +16274,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A131" s="6"/>
       <c r="B131" s="5">
         <v>3</v>
@@ -16621,7 +16624,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="150" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A145" s="6"/>
       <c r="B145" s="5">
         <v>3</v>
@@ -16646,7 +16649,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A146" s="6"/>
       <c r="B146" s="5">
         <v>3</v>
@@ -16771,7 +16774,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A151" s="6"/>
       <c r="B151" s="5">
         <v>3</v>
@@ -16796,7 +16799,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A152" s="6"/>
       <c r="B152" s="5">
         <v>3</v>
@@ -16821,7 +16824,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A153" s="6"/>
       <c r="B153" s="5">
         <v>3</v>
@@ -16896,7 +16899,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="328" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A156" s="6"/>
       <c r="B156" s="5">
         <v>3</v>
@@ -16921,7 +16924,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A157" s="6"/>
       <c r="B157" s="5">
         <v>3</v>
@@ -16971,7 +16974,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A159" s="6"/>
       <c r="B159" s="5">
         <v>3</v>
@@ -16996,7 +16999,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="195" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" ht="165" x14ac:dyDescent="0.2">
       <c r="A160" s="6"/>
       <c r="B160" s="5">
         <v>3</v>
@@ -17021,7 +17024,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="225" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A161" s="6"/>
       <c r="B161" s="5">
         <v>3</v>
@@ -17096,7 +17099,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" ht="195" x14ac:dyDescent="0.2">
       <c r="A164" s="6"/>
       <c r="B164" s="5">
         <v>3</v>
@@ -17146,7 +17149,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="195" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A166" s="6"/>
       <c r="B166" s="5">
         <v>3</v>
@@ -17271,7 +17274,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="300" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A171" s="6"/>
       <c r="B171" s="5">
         <v>3</v>
@@ -17296,7 +17299,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A172" s="6"/>
       <c r="B172" s="5">
         <v>3</v>
@@ -17321,7 +17324,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A173" s="6"/>
       <c r="B173" s="5">
         <v>3</v>
@@ -17346,7 +17349,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A174" s="6"/>
       <c r="B174" s="5">
         <v>3</v>
@@ -17371,7 +17374,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A175" s="6"/>
       <c r="B175" s="5">
         <v>3</v>
@@ -17496,7 +17499,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="180" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A180" s="6"/>
       <c r="B180" s="5">
         <v>3</v>
@@ -17521,7 +17524,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A181" s="6"/>
       <c r="B181" s="5">
         <v>3</v>
@@ -17727,7 +17730,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A189" s="6"/>
       <c r="B189" s="5">
         <v>1</v>
@@ -17839,7 +17842,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A193" s="6" t="s">
         <v>1011</v>
       </c>
@@ -17866,7 +17869,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A194" s="6"/>
       <c r="B194" s="7">
         <v>4</v>
@@ -17889,7 +17892,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A195" s="6" t="s">
         <v>1011</v>
       </c>
@@ -17916,7 +17919,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" ht="270" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18132,7 +18135,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" ht="165" x14ac:dyDescent="0.2">
       <c r="A204" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18290,7 +18293,7 @@
       </c>
       <c r="L209" s="17"/>
     </row>
-    <row r="210" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A210" s="6"/>
       <c r="B210" s="7">
         <v>3</v>
@@ -18483,7 +18486,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18537,7 +18540,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18645,7 +18648,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A223" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18672,7 +18675,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A224" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18726,7 +18729,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A226" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18807,7 +18810,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="229" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A229" s="6"/>
       <c r="B229" s="7">
         <v>3</v>
@@ -18838,7 +18841,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="230" spans="1:12" ht="285" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A230" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18863,7 +18866,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="231" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
         <v>1011</v>
       </c>
@@ -18890,7 +18893,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="232" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19276,7 +19279,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="246" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A246" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19303,7 +19306,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="247" spans="1:12" ht="105" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A247" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19411,7 +19414,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="251" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:12" ht="165" x14ac:dyDescent="0.2">
       <c r="A251" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19708,7 +19711,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="225" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A262" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19760,7 +19763,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="264" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A264" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19814,7 +19817,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="266" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A266" s="6"/>
       <c r="B266" s="7">
         <v>3</v>
@@ -19872,7 +19875,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A268" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19899,7 +19902,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="269" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A269" s="6" t="s">
         <v>1011</v>
       </c>
@@ -19926,7 +19929,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="270" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A270" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20115,7 +20118,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="277" spans="1:12" ht="150" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A277" s="6"/>
       <c r="B277" s="7">
         <v>4</v>
@@ -20167,7 +20170,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="279" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A279" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20271,7 +20274,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12" ht="370" x14ac:dyDescent="0.2">
       <c r="A283" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20298,7 +20301,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="284" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A284" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20325,7 +20328,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A285" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20620,7 +20623,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="296" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A296" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20647,7 +20650,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="297" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A297" s="6"/>
       <c r="B297" s="7">
         <v>4</v>
@@ -20670,7 +20673,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="298" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A298" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20724,7 +20727,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="300" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A300" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20890,7 +20893,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="306" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:12" ht="370" x14ac:dyDescent="0.2">
       <c r="A306" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20915,7 +20918,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="307" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A307" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20940,7 +20943,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="308" spans="1:12" ht="225" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A308" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20967,7 +20970,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="309" spans="1:12" ht="150" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A309" s="6" t="s">
         <v>1011</v>
       </c>
@@ -20994,7 +20997,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="310" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A310" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21021,7 +21024,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="311" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A311" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21271,7 +21274,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="320" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A320" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21298,7 +21301,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="321" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A321" s="6"/>
       <c r="B321" s="7">
         <v>3</v>
@@ -21352,7 +21355,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="323" spans="1:12" ht="105" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A323" s="6"/>
       <c r="B323" s="7">
         <v>3</v>
@@ -21410,7 +21413,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="325" spans="1:12" ht="195" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A325" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21516,7 +21519,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="329" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A329" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21597,7 +21600,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="332" spans="1:12" ht="270" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A332" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21703,7 +21706,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="336" spans="1:12" ht="135" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:12" ht="105" x14ac:dyDescent="0.2">
       <c r="A336" s="6"/>
       <c r="B336" s="7">
         <v>1</v>
@@ -21734,7 +21737,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="337" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A337" s="6"/>
       <c r="B337" s="7">
         <v>2</v>
@@ -21819,7 +21822,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="340" spans="1:12" ht="150" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A340" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21900,7 +21903,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="343" spans="1:12" ht="225" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:12" ht="195" x14ac:dyDescent="0.2">
       <c r="A343" s="6" t="s">
         <v>1011</v>
       </c>
@@ -21981,7 +21984,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="346" spans="1:12" ht="328" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A346" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22008,7 +22011,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="347" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:12" ht="105" x14ac:dyDescent="0.2">
       <c r="A347" s="6"/>
       <c r="B347" s="7">
         <v>2</v>
@@ -22039,7 +22042,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="348" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A348" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22066,7 +22069,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="349" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A349" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22093,7 +22096,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="350" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A350" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22147,7 +22150,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="352" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A352" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22174,7 +22177,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="353" spans="1:12" ht="195" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A353" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22201,7 +22204,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="354" spans="1:12" ht="300" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A354" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22305,7 +22308,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="358" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:12" ht="195" x14ac:dyDescent="0.2">
       <c r="A358" s="6"/>
       <c r="B358" s="7">
         <v>2</v>
@@ -22336,7 +22339,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="359" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A359" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22538,7 +22541,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="367" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A367" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22590,7 +22593,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="369" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A369" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22615,7 +22618,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="370" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A370" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22696,7 +22699,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="373" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A373" s="6" t="s">
         <v>1011</v>
       </c>
@@ -22828,7 +22831,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="378" spans="1:12" ht="135" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A378" s="6"/>
       <c r="B378" s="7">
         <v>2</v>
@@ -22884,7 +22887,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="380" spans="1:12" ht="135" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:12" ht="105" x14ac:dyDescent="0.2">
       <c r="A380" s="6"/>
       <c r="B380" s="7">
         <v>2</v>
@@ -22965,7 +22968,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="383" spans="1:12" ht="300" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A383" s="6"/>
       <c r="B383" s="7">
         <v>3</v>
@@ -23071,7 +23074,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="387" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A387" s="6"/>
       <c r="B387" s="7">
         <v>3</v>
@@ -23349,7 +23352,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="397" spans="1:12" ht="384" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A397" s="6" t="s">
         <v>1011</v>
       </c>
@@ -23376,7 +23379,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="398" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A398" s="6"/>
       <c r="B398" s="7">
         <v>2</v>
@@ -23488,7 +23491,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="402" spans="1:12" ht="225" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A402" s="6"/>
       <c r="B402" s="7">
         <v>2</v>
@@ -23702,7 +23705,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="410" spans="1:12" ht="285" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A410" s="6" t="s">
         <v>1011</v>
       </c>
@@ -23808,7 +23811,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="414" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A414" s="6" t="s">
         <v>1011</v>
       </c>
@@ -23983,7 +23986,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="421" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A421" s="6"/>
       <c r="B421" s="7">
         <v>2</v>
@@ -24014,7 +24017,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="422" spans="1:12" ht="225" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:12" ht="210" x14ac:dyDescent="0.2">
       <c r="A422" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24149,7 +24152,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="427" spans="1:12" ht="300" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:12" ht="285" x14ac:dyDescent="0.2">
       <c r="A427" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24176,7 +24179,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="428" spans="1:12" ht="285" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:12" ht="270" x14ac:dyDescent="0.2">
       <c r="A428" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24203,7 +24206,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="429" spans="1:12" ht="328" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A429" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24230,7 +24233,7 @@
         <v>2217</v>
       </c>
     </row>
-    <row r="430" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A430" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24404,7 +24407,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="436" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A436" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24458,7 +24461,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="438" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:12" ht="225" x14ac:dyDescent="0.2">
       <c r="A438" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24593,7 +24596,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="443" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A443" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24668,7 +24671,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="446" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A446" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24693,7 +24696,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="447" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A447" s="6"/>
       <c r="B447" s="7">
         <v>4</v>
@@ -24772,7 +24775,7 @@
         <v>2317</v>
       </c>
     </row>
-    <row r="450" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A450" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24826,7 +24829,7 @@
         <v>2327</v>
       </c>
     </row>
-    <row r="452" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A452" s="6" t="s">
         <v>1011</v>
       </c>
@@ -24932,7 +24935,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="456" spans="1:12" ht="270" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A456" s="6"/>
       <c r="B456" s="7">
         <v>4</v>
@@ -24957,7 +24960,7 @@
         <v>2351</v>
       </c>
     </row>
-    <row r="457" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:12" ht="240" x14ac:dyDescent="0.2">
       <c r="A457" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25038,7 +25041,7 @@
         <v>2366</v>
       </c>
     </row>
-    <row r="460" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:12" ht="270" x14ac:dyDescent="0.2">
       <c r="A460" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25092,7 +25095,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="462" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A462" s="6"/>
       <c r="B462" s="7">
         <v>4</v>
@@ -25115,7 +25118,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="463" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A463" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25142,7 +25145,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="464" spans="1:12" ht="105" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A464" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25196,7 +25199,7 @@
         <v>2395</v>
       </c>
     </row>
-    <row r="466" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A466" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25246,7 +25249,7 @@
         <v>2403</v>
       </c>
     </row>
-    <row r="468" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A468" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25558,7 +25561,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="480" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A480" s="6"/>
       <c r="B480" s="7">
         <v>3</v>
@@ -25616,7 +25619,7 @@
         <v>2472</v>
       </c>
     </row>
-    <row r="482" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:12" ht="165" x14ac:dyDescent="0.2">
       <c r="A482" s="6"/>
       <c r="B482" s="7">
         <v>4</v>
@@ -25776,7 +25779,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="488" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A488" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25803,7 +25806,7 @@
         <v>2507</v>
       </c>
     </row>
-    <row r="489" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A489" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25830,7 +25833,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="490" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A490" s="6" t="s">
         <v>1011</v>
       </c>
@@ -25990,7 +25993,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="496" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A496" s="6" t="s">
         <v>1011</v>
       </c>
@@ -26071,7 +26074,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="499" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:12" ht="150" x14ac:dyDescent="0.2">
       <c r="A499" s="6" t="s">
         <v>1011</v>
       </c>
@@ -26098,7 +26101,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="500" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A500" s="6" t="s">
         <v>1011</v>
       </c>
@@ -26125,7 +26128,7 @@
         <v>2567</v>
       </c>
     </row>
-    <row r="501" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:12" ht="195" x14ac:dyDescent="0.2">
       <c r="A501" s="6" t="s">
         <v>1011</v>
       </c>
@@ -26179,7 +26182,7 @@
         <v>2577</v>
       </c>
     </row>
-    <row r="503" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A503" s="6" t="s">
         <v>1011</v>
       </c>
@@ -26422,7 +26425,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="512" spans="1:12" ht="314" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A512" s="6"/>
       <c r="B512" s="7">
         <v>4</v>
@@ -26447,7 +26450,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="513" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A513" s="6"/>
       <c r="B513" s="7">
         <v>4</v>
@@ -26497,7 +26500,7 @@
         <v>2637</v>
       </c>
     </row>
-    <row r="515" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A515" s="6"/>
       <c r="B515" s="7">
         <v>4</v>
@@ -26522,7 +26525,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="516" spans="1:12" ht="270" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A516" s="6"/>
       <c r="B516" s="7">
         <v>4</v>
@@ -26572,7 +26575,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="518" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:12" ht="300" x14ac:dyDescent="0.2">
       <c r="A518" s="6"/>
       <c r="B518" s="7">
         <v>4</v>
@@ -26672,7 +26675,7 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="522" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A522" s="6"/>
       <c r="B522" s="7">
         <v>4</v>
@@ -26697,7 +26700,7 @@
         <v>2677</v>
       </c>
     </row>
-    <row r="523" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A523" s="6"/>
       <c r="B523" s="7">
         <v>3</v>
@@ -27471,7 +27474,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="553" spans="1:12" ht="398" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:12" ht="384" x14ac:dyDescent="0.2">
       <c r="A553" s="6"/>
       <c r="B553" s="7">
         <v>4</v>
@@ -27521,7 +27524,7 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="555" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:12" ht="105" x14ac:dyDescent="0.2">
       <c r="A555" s="6"/>
       <c r="B555" s="7">
         <v>3</v>
@@ -27627,7 +27630,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="559" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A559" s="6"/>
       <c r="B559" s="7">
         <v>3</v>
@@ -27783,7 +27786,7 @@
         <v>2899</v>
       </c>
     </row>
-    <row r="565" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A565" s="6"/>
       <c r="B565" s="7">
         <v>3</v>
@@ -27939,7 +27942,7 @@
         <v>2931</v>
       </c>
     </row>
-    <row r="571" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A571" s="6"/>
       <c r="B571" s="7">
         <v>3</v>
@@ -28020,7 +28023,7 @@
         <v>2947</v>
       </c>
     </row>
-    <row r="574" spans="1:12" ht="370" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A574" s="6"/>
       <c r="B574" s="7">
         <v>4</v>
@@ -28145,7 +28148,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="579" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A579" s="6"/>
       <c r="B579" s="7">
         <v>3</v>
@@ -28176,7 +28179,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="580" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A580" s="6"/>
       <c r="B580" s="7">
         <v>4</v>
@@ -28276,7 +28279,7 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="584" spans="1:12" ht="150" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A584" s="6"/>
       <c r="B584" s="7">
         <v>3</v>
@@ -28357,7 +28360,7 @@
         <v>3016</v>
       </c>
     </row>
-    <row r="587" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A587" s="6"/>
       <c r="B587" s="7">
         <v>3</v>
@@ -28638,7 +28641,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="598" spans="1:12" ht="384" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:12" ht="356" x14ac:dyDescent="0.2">
       <c r="A598" s="6"/>
       <c r="B598" s="7">
         <v>4</v>
@@ -28719,7 +28722,7 @@
         <v>3090</v>
       </c>
     </row>
-    <row r="601" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A601" s="6"/>
       <c r="B601" s="7">
         <v>4</v>
@@ -28825,7 +28828,7 @@
         <v>3112</v>
       </c>
     </row>
-    <row r="605" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A605" s="6"/>
       <c r="B605" s="7">
         <v>1</v>
@@ -28856,7 +28859,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="606" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A606" s="6"/>
       <c r="B606" s="7">
         <v>2</v>
@@ -29047,7 +29050,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="613" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A613" s="6"/>
       <c r="B613" s="7">
         <v>1</v>
@@ -29078,7 +29081,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="614" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A614" s="6"/>
       <c r="B614" s="7">
         <v>2</v>
@@ -29134,7 +29137,7 @@
         <v>3173</v>
       </c>
     </row>
-    <row r="616" spans="1:12" ht="165" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A616" s="6"/>
       <c r="B616" s="5">
         <v>2</v>
@@ -29190,7 +29193,7 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="618" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A618" s="6"/>
       <c r="B618" s="5">
         <v>3</v>
@@ -29265,7 +29268,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="621" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A621" s="6"/>
       <c r="B621" s="5">
         <v>2</v>
@@ -29296,7 +29299,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="622" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A622" s="6"/>
       <c r="B622" s="5">
         <v>3</v>
@@ -29458,7 +29461,7 @@
         <v>3241</v>
       </c>
     </row>
-    <row r="628" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A628" s="6"/>
       <c r="B628" s="5">
         <v>3</v>
@@ -29720,7 +29723,7 @@
         <v>3295</v>
       </c>
     </row>
-    <row r="638" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:12" ht="328" x14ac:dyDescent="0.2">
       <c r="A638" s="6"/>
       <c r="B638" s="5">
         <v>3</v>
@@ -29857,7 +29860,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="643" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="643" spans="1:12" ht="398" x14ac:dyDescent="0.2">
       <c r="A643" s="6"/>
       <c r="B643" s="5">
         <v>3</v>
@@ -29932,7 +29935,7 @@
         <v>3339</v>
       </c>
     </row>
-    <row r="646" spans="1:12" ht="342" x14ac:dyDescent="0.2">
+    <row r="646" spans="1:12" ht="314" x14ac:dyDescent="0.2">
       <c r="A646" s="6"/>
       <c r="B646" s="5">
         <v>3</v>
@@ -30281,7 +30284,7 @@
         <v>3413</v>
       </c>
     </row>
-    <row r="659" spans="1:12" ht="210" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A659" s="6"/>
       <c r="B659" s="5">
         <v>3</v>
@@ -30356,7 +30359,7 @@
         <v>3428</v>
       </c>
     </row>
-    <row r="662" spans="1:12" ht="384" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:12" ht="342" x14ac:dyDescent="0.2">
       <c r="A662" s="6"/>
       <c r="B662" s="5">
         <v>3</v>
@@ -31029,6 +31032,7 @@
       <c r="D700" s="57"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L683" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>